<commit_message>
changes of the code to abstract it
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,297 +429,342 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>Introduction to Computer Science Principles I</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Jessie Carbajal-Rivas (Primary)</t>
-        </is>
-      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Monday-Tuesday-Wednesday-Thursday-Friday , 02:00 PM - 03:00 PM</t>
+          <t>Joshua Cormier (Primary)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>10 of 30 seats remain.</t>
+          <t>Monday-Tuesday-Wednesday-Thursday-Friday , 08:49 AM - 09:34 AM</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>16 of 20 seats remain.</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>1110</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Introduction to Computer Science Principles I</t>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>Introduction to Computer Science Principles II</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>Andrew Lapetina (Primary)</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Monday-Tuesday-Wednesday-Thursday-Friday , 12:15 PM - 01:10 PM</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>10 of 30 seats remain.</t>
+          <t>Monday-Tuesday-Wednesday-Thursday-Friday , 09:46 AM - 10:39 AM</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>22 of 35 seats remain.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>1110</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Introduction to Computer Science Principles I</t>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Andrew Lapetina (Primary)</t>
+          <t>Introduction to Computer Science Principles II</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Monday-Tuesday-Wednesday-Thursday-Friday , 01:50 PM - 02:50 PM</t>
+          <t>Liz Roberts-Kirchhoff (Primary)
+Jessie Carbajal-Rivas</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>4 of 30 seats remain.</t>
+          <t>Monday-Tuesday-Wednesday-Thursday-Friday , 10:45 AM - 11:45 AM</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>20 of 35 seats remain.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>1110</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Introduction to Computer Science Principles I</t>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Terry Laesser (Primary)</t>
+          <t>Introduction to Computer Science Principles II</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Monday-Tuesday-Wednesday-Thursday-Friday , 11:45 AM - 12:45 PM</t>
+          <t>Liz Roberts-Kirchhoff (Primary)
+Jessie Carbajal-Rivas</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>15 of 40 seats remain.</t>
+          <t>Monday-Tuesday-Wednesday-Thursday-Friday , 12:55 PM - 01:55 PM</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>15 of 35 seats remain.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>1110</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Introduction to Computer Science Principles I</t>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>Introduction to Computer Science Principles II</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Andrew Lapetina (Primary)</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Monday-Tuesday-Wednesday-Thursday-Friday , 09:05 AM - 10:05 AM</t>
-        </is>
-      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>14 of 30 seats remain.</t>
+          <t>Tuesday-Wednesday-Thursday-Friday , 01:23 PM - 02:11 PM</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>16 of 35 seats remain.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>1110</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Introduction to Computer Science Principles I</t>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Andrew Lapetina (Primary)</t>
+          <t>Introduction to Computer Science Principles II</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Monday-Tuesday-Wednesday-Thursday-Friday , 10:10 AM - 11:10 AM</t>
+          <t>Liz Roberts-Kirchhoff (Primary)
+Michael Mitchell
+Andrew Lapetina</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>18 of 30 seats remain.</t>
+          <t>Monday-Tuesday-Wednesday-Thursday-Friday , 01:50 PM - 02:50 PM</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>22 of 35 seats remain.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1710</t>
+          <t>1110</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Introduction to Programming I</t>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Tarek Dakhlallah (Primary)</t>
+          <t>Introduction to Computer Science Principles II</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Tuesday-Thursday , 11:20 AM - 12:35 PM</t>
+          <t>Liz Roberts-Kirchhoff (Primary)
+Terry Laesser</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>4 of 28 seats remain.</t>
+          <t>Monday-Tuesday-Wednesday-Thursday-Friday , 12:39 PM - 01:34 PM</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>25 of 35 seats remain.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1710</t>
+          <t>1110</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Associated Term:Fall 2022
-CRN:18021
-Campus:On-Line
-Schedule Type: Online 100%
-Instructional Method: Online 100%
-Section Number: CE1
-Subject: Comp Sci/Software Engineering
-Course Number: 1710
-Title: Introduction to Programming I
-Credit Hours: 3
-Grade Mode: No Section specified grade mode, please see Catalog link below for more information.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Introduction to Programming I</t>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Shadi Bedoor (Primary)</t>
+          <t>Introduction to Computer Science Principles II</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>55 of 100 seats remain.</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>Andrew Lapetina (Primary)</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Monday-Tuesday-Wednesday-Thursday-Friday , 11:15 AM - 12:15 PM</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>27 of 35 seats remain.</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1710</t>
+          <t>1110</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Introduction to Programming I</t>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Shadi Bedoor (Primary)</t>
+          <t>Introduction to Computer Science Principles II</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Thursday-Friday , 05:40 AM - 07:15 AM</t>
+          <t>Joshua Cormier (Primary)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>11 of 100 seats remain.</t>
+          <t>Monday-Tuesday-Wednesday-Thursday-Friday , 08:00 AM - 08:45 AM</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>6 of 20 seats remain.</t>
         </is>
       </c>
     </row>
@@ -731,449 +776,632 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>Introduction to Programming I</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Shadi Bedoor (Primary)</t>
-        </is>
-      </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>33 of 100 seats remain.</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
+          <t>Mina Maleki (Primary)</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Tuesday-Thursday , 11:20 AM - 12:35 PM</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>16 of 30 seats remain.</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1710</t>
+          <t>1711</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Introduction to Programming I</t>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Shadi Bedoor (Primary)</t>
+          <t>Programming I Laboratory</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>40 of 100 seats remain.</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
+          <t>Mina Maleki (Primary)</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Tuesday , 05:15 PM - 06:30 PM</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>FULL: 0 of 12 seats remain.
+8 of 8 waitlist seats remain.</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1710</t>
+          <t>1711</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Associated Term:Fall 2022
-CRN:17762
-Campus:Univ of Detroit Jesuit HS
-Schedule Type: Lab/Lecture
-Instructional Method: Traditional
-Section Number: UD
-Subject: Comp Sci/Software Engineering
-Course Number: 1710
-Title: Introduction to Programming I
-Credit Hours: 3
-Grade Mode: No Section specified grade mode, please see Catalog link below for more information.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Introduction to Programming I</t>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Clarence Wilson (Primary)</t>
+          <t>Programming I Laboratory</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Monday-Tuesday-Wednesday-Thursday-Friday , 10:41 AM - 11:26 AM</t>
+          <t>Hebah Alquran (Primary)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>10 of 20 seats remain.</t>
-        </is>
-      </c>
+          <t>18 of 20 seats remain.</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1711</t>
+          <t>1720</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>['1710,C']</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Programming I Laboratory</t>
+          <t xml:space="preserve">Catalog Prerequisites
+Area Prerequisites
+Prerequisites:Prereq(s) for CSSE1720 are:
+ Course or Test: Comp Sci/Software Engineering 1710 
+ Minimum Grade of C
+ May not be taken concurrently. </t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Tarek Dakhlallah (Primary)</t>
+          <t>Introduction to Programming II</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Wednesday , 02:00 PM - 03:15 PM</t>
+          <t>Shadi Elaiyan Bani Taan (Primary)</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>1 of 12 seats remain.</t>
+          <t>Monday-Wednesday , 12:30 PM - 01:45 PM</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>4 of 20 seats remain.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1711</t>
+          <t>1720</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>['1710,C']</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Programming I Laboratory</t>
+          <t xml:space="preserve">Catalog Prerequisites
+Area Prerequisites
+Prerequisites:Prereq(s) for CSSE1720 are:
+ Course or Test: Comp Sci/Software Engineering 1710 
+ Minimum Grade of C
+ May not be taken concurrently. </t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Tarek Dakhlallah (Primary)</t>
+          <t>Introduction to Programming II</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Thursday , 03:30 PM - 04:45 PM</t>
+          <t>Raef Aidibi (Primary)</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>3 of 12 seats remain.</t>
+          <t>Monday-Wednesday , 12:30 PM - 01:45 PM</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>8 of 24 seats remain.
+10 of 10 waitlist seats remain.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2130</t>
+          <t>1720</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Associated Term:Fall 2022
-CRN:14427
-Campus:McNichols Campus
-Schedule Type: Lecture
-Instructional Method: Traditional
-Section Number: 01
-Subject: Comp Sci/Software Engineering
-Course Number: 2130
-Title: Java
-Credit Hours: 3
-Grade Mode: No Section specified grade mode, please see Catalog link below for more information.</t>
+          <t>['1710,C']</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Java</t>
+          <t xml:space="preserve">Catalog Prerequisites
+Area Prerequisites
+Prerequisites:Prereq(s) for CSSE1720 are:
+ Course or Test: Comp Sci/Software Engineering 1710 
+ Minimum Grade of C
+ May not be taken concurrently. </t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Mina Maleki (Primary)</t>
+          <t>Introduction to Programming II</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Tuesday-Thursday , 02:00 PM - 03:15 PM</t>
+          <t>Ahmad Aljaafreh (Primary)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>6 of 20 seats remain.</t>
+          <t>Monday-Wednesday , 08:00 AM - 10:00 AM</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>FULL: 0 of 100 seats remain.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2130</t>
+          <t>1720</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Associated Term:Fall 2022
-CRN:18015
-Campus:On-Line
-Schedule Type: Online 100%
-Instructional Method: Online 100%
-Section Number: SE1
-Subject: Comp Sci/Software Engineering
-Course Number: 2130
-Title: Java
-Credit Hours: 3
-Grade Mode: No Section specified grade mode, please see Catalog link below for more information.</t>
+          <t>['1710,C']</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Java</t>
+          <t xml:space="preserve">Catalog Prerequisites
+Area Prerequisites
+Prerequisites:Prereq(s) for CSSE1720 are:
+ Course or Test: Comp Sci/Software Engineering 1710 
+ Minimum Grade of C
+ May not be taken concurrently. </t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Omid Aghili (Primary)</t>
+          <t>Introduction to Programming II</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>36 of 100 seats remain.</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr"/>
+          <t>Ahmad Aljaafreh (Primary)</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Tuesday-Thursday , 07:00 PM - 09:45 PM</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>31 of 100 seats remain.</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>3430</t>
+          <t>1721</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Associated Term:Fall 2022
-CRN:15599
-Campus:McNichols Campus
-Schedule Type: Lecture
-Instructional Method: Traditional
-Section Number: 01
-Subject: Comp Sci/Software Engineering
-Course Number: 3430
-Title: Data Structures
-Credit Hours: 3
-Grade Mode: No Section specified grade mode, please see Catalog link below for more information.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Data Structures</t>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Mina Maleki (Primary)</t>
+          <t>Programming II Laboratory</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Tuesday-Thursday , 11:20 AM - 12:35 PM</t>
+          <t>Shadi Elaiyan Bani Taan (Primary)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>4 of 20 seats remain.</t>
+          <t>Wednesday , 02:00 PM - 03:15 PM</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>1 of 13 seats remain.
+5 of 5 waitlist seats remain.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>3430</t>
+          <t>1721</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Associated Term:Fall 2022
-CRN:18016
-Campus:On-Line
-Schedule Type: Online 100%
-Instructional Method: Online 100%
-Section Number: EE1
-Subject: Comp Sci/Software Engineering
-Course Number: 3430
-Title: Data Structures
-Credit Hours: 3
-Grade Mode: No Section specified grade mode, please see Catalog link below for more information.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Data Structures</t>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Omid Aghili (Primary)</t>
+          <t>Programming II Laboratory</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>12 of 100 seats remain.</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr"/>
+          <t>Shadi Elaiyan Bani Taan (Primary)</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Monday , 02:00 PM - 03:15 PM</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>3 of 13 seats remain.
+5 of 5 waitlist seats remain.</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>3430</t>
+          <t>3540</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Associated Term:Fall 2022
-CRN:18017
-Campus:On-Line
-Schedule Type: Online 100%
-Instructional Method: Online 100%
-Section Number: SE1
-Subject: Comp Sci/Software Engineering
-Course Number: 3430
-Title: Data Structures
-Credit Hours: 3
-Grade Mode: No Section specified grade mode, please see Catalog link below for more information.</t>
+          <t>['1720,C', 'or', '1722,C']</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Data Structures</t>
+          <t>Catalog Prerequisites
+Area Prerequisites
+Prerequisites:Prereq(s) for CSSE3540 are:
+(
+ Course or Test: Comp Sci/Software Engineering 1720 
+ Minimum Grade of C
+ May not be taken concurrently. 
+)
+or
+(
+ Course or Test: Comp Sci/Software Engineering 1722 
+ Minimum Grade of C
+ May not be taken concurrently. 
+)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Omid Aghili (Primary)</t>
+          <t>Database Systems and Programming</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>36 of 100 seats remain.</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr"/>
+          <t>Mina Maleki (Primary)</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Tuesday-Thursday , 02:00 PM - 03:15 PM</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>7 of 20 seats remain.</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4150</t>
+          <t>4440</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Associated Term:Fall 2022
-CRN:13488
-Campus:McNichols Campus
-Schedule Type: Lecture
-Instructional Method: Traditional
-Section Number: 01
-Subject: Comp Sci/Software Engineering
-Course Number: 4150
-Title: Introduction to Software Engineering
-Credit Hours: 3
-Grade Mode: No Section specified grade mode, please see Catalog link below for more information.</t>
+          <t>['1720,C', 'or', '1722,C']</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Introduction to Software Engineering</t>
+          <t>Catalog Prerequisites
+Area Prerequisites
+Prerequisites:Prereq(s) for CSSE4440 are:
+(
+ Course or Test: Comp Sci/Software Engineering 1720 
+ Minimum Grade of C
+ May not be taken concurrently. 
+)
+or
+(
+ Course or Test: Comp Sci/Software Engineering 1722 
+ Minimum Grade of C
+ May not be taken concurrently. 
+)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Mina Maleki (Primary)</t>
+          <t>Web Technology</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Tuesday-Thursday , 03:30 PM - 04:45 PM</t>
+          <t>Omid Aghili (Primary)</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>16 of 20 seats remain.</t>
+          <t>Monday-Wednesday , 01:30 PM - 04:45 PM</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>43 of 100 seats remain.</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4540</t>
+          <t>4490</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Associated Term:Fall 2022
-CRN:17746
-Campus:On-Line
-Schedule Type: Online 100%
-Instructional Method: Online 100%
-Section Number: OL
-Subject: Comp Sci/Software Engineering
-Course Number: 4540
-Title: Computer Security
-Credit Hours: 3
-Grade Mode: No Section specified grade mode, please see Catalog link below for more information.</t>
+          <t>['3430,C']</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Computer Security</t>
+          <t xml:space="preserve">Catalog Prerequisites
+Area Prerequisites
+Prerequisites:Prereq(s) for CSSE4490 are:
+ Course or Test: Comp Sci/Software Engineering 3430 
+ Minimum Grade of C
+ May not be taken concurrently. </t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Mustafa Saed (Primary)</t>
+          <t>Operating Systems</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>17 of 20 seats remain.</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr"/>
+          <t>Abhijit Dasgupta (Primary)</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Monday-Wednesday , 05:15 PM - 06:30 PM</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>24 of 34 seats remain.</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>4540</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Computer Security</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Omid Aghili (Primary)</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Tuesday-Thursday , 01:30 PM - 04:45 PM</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>43 of 100 seats remain.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>4550</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>['3430,C']</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Catalog Prerequisites
+Area Prerequisites
+Prerequisites:Prereq(s) for CSSE4550 are:
+ Course or Test: Comp Sci/Software Engineering 3430 
+ Minimum Grade of C
+ May not be taken concurrently. </t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Introduction to Artificial Intelligence</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Shadi Elaiyan Bani Taan (Primary)</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Monday-Wednesday , 11:00 AM - 12:15 PM</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>14 of 20 seats remain.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>4550</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>['3430,C']</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Catalog Prerequisites
+Area Prerequisites
+Prerequisites:Prereq(s) for CSSE4550 are:
+ Course or Test: Comp Sci/Software Engineering 3430 
+ Minimum Grade of C
+ May not be taken concurrently. </t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Introduction to Artificial Intelligence</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Omid Aghili (Primary)</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Tuesday-Thursday , 06:00 PM - 08:55 PM</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>42 of 100 seats remain.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
           <t>4570</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>['4150,C']</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
         <is>
           <t xml:space="preserve">Catalog Prerequisites
 Area Prerequisites
@@ -1183,256 +1411,284 @@
  May not be taken concurrently. </t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>Software Project Management</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>Kevin Daimi (Primary)</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Tuesday-Thursday , 02:00 PM - 03:15 PM</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>12 of 20 seats remain.</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>4610</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Associated Term:Fall 2022
-CRN:17105
-Campus:McNichols Campus
-Schedule Type: Lecture
-Instructional Method: Traditional
-Section Number: 01
-Subject: Comp Sci/Software Engineering
-Course Number: 4610
-Title: Introduction to Data Mining
-Credit Hours: 3
-Grade Mode: No Section specified grade mode, please see Catalog link below for more information.</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Introduction to Data Mining</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Shadi Elaiyan Bani Taan (Primary)</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Monday-Wednesday , 10:00 AM - 11:15 AM</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>9 of 12 seats remain.
-5 of 5 waitlist seats remain.</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>4951</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Senior Design Project I</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Shadi Elaiyan Bani Taan (Primary)</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Monday , 01:00 PM - 03:30 PM</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>12 of 20 seats remain.</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>5120</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Introduction to Data Science</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Matt Haley (Primary)</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>18 of 20 seats remain.</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>14 of 25 seats remain.</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5150</t>
+          <t>4900</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Software Engineering</t>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Mina Maleki (Primary)</t>
+          <t>Game Design, Develop, &amp; Tools</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Tuesday-Thursday , 03:30 PM - 04:45 PM</t>
+          <t>Steven Rice (Primary)</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>18 of 20 seats remain.</t>
+          <t>Monday-Wednesday , 02:00 PM - 03:15 PM</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>FULL: 0 of 20 seats remain.</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5310</t>
+          <t>4952</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>['4951,C']</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Data Mining</t>
+          <t xml:space="preserve">Catalog Prerequisites
+Area Prerequisites
+Prerequisites:Prereq(s) for CSSE4952 are:
+ Course or Test: Comp Sci/Software Engineering 4951 
+ Minimum Grade of C
+ May not be taken concurrently. </t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
+          <t>Senior Design Project II</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
           <t>Shadi Elaiyan Bani Taan (Primary)</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Monday-Wednesday , 10:00 AM - 11:15 AM</t>
-        </is>
-      </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>7 of 8 seats remain.
-5 of 5 waitlist seats remain.</t>
+          <t>Monday-Wednesday , 09:00 AM - 10:15 AM</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>13 of 20 seats remain.</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5520</t>
+          <t>5480</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Architectures for Software Systems</t>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Rita Barrios (Primary)</t>
+          <t>Artificial Intelligence</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>25 of 30 seats remain.</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr"/>
+          <t>Shadi Elaiyan Bani Taan (Primary)</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Monday-Wednesday , 11:00 AM - 12:15 PM</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>8 of 20 seats remain.</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5760</t>
+          <t>5520</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Network Security</t>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Sakhr Youness (Primary)</t>
+          <t>Architectures for Software Systems</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>12 of 20 seats remain.</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr"/>
+          <t>Rita Barrios (Primary)</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>18 of 25 seats remain.</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>5550</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Software Requirements Engineering</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Mina Maleki (Primary)</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Tuesday-Thursday , 03:30 PM - 04:45 PM</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>14 of 20 seats remain.</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>5570</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Software Systems Project Management</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Kevin Daimi (Primary)</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>22 of 25 seats remain.</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>5930</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Catalog Prerequisites
+No prerequisite information available.</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Graduate Design Project</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Shadi Elaiyan Bani Taan (Primary)</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> , -</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>1 of 5 seats remain.</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
get the list of courses
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,33 +429,17 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Introduction to Computer Science Principles I</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Introduction to Computer Science Principles I</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Joshua Cormier (Primary)</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
           <t>Monday-Tuesday-Wednesday-Thursday-Friday , 08:49 AM - 09:34 AM</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>16 of 20 seats remain.</t>
         </is>
       </c>
     </row>
@@ -467,33 +451,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Introduction to Computer Science Principles II</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Introduction to Computer Science Principles II</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Andrew Lapetina (Primary)</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
           <t>Monday-Tuesday-Wednesday-Thursday-Friday , 09:46 AM - 10:39 AM</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>22 of 35 seats remain.</t>
         </is>
       </c>
     </row>
@@ -505,34 +473,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Introduction to Computer Science Principles II</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Introduction to Computer Science Principles II</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Liz Roberts-Kirchhoff (Primary)
-Jessie Carbajal-Rivas</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
           <t>Monday-Tuesday-Wednesday-Thursday-Friday , 10:45 AM - 11:45 AM</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>20 of 35 seats remain.</t>
         </is>
       </c>
     </row>
@@ -544,34 +495,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Introduction to Computer Science Principles II</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Introduction to Computer Science Principles II</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Liz Roberts-Kirchhoff (Primary)
-Jessie Carbajal-Rivas</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
           <t>Monday-Tuesday-Wednesday-Thursday-Friday , 12:55 PM - 01:55 PM</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>15 of 35 seats remain.</t>
         </is>
       </c>
     </row>
@@ -583,33 +517,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Introduction to Computer Science Principles II</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Introduction to Computer Science Principles II</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Andrew Lapetina (Primary)</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
           <t>Tuesday-Wednesday-Thursday-Friday , 01:23 PM - 02:11 PM</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>16 of 35 seats remain.</t>
         </is>
       </c>
     </row>
@@ -621,35 +539,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Introduction to Computer Science Principles II</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Introduction to Computer Science Principles II</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Liz Roberts-Kirchhoff (Primary)
-Michael Mitchell
-Andrew Lapetina</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
           <t>Monday-Tuesday-Wednesday-Thursday-Friday , 01:50 PM - 02:50 PM</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>22 of 35 seats remain.</t>
         </is>
       </c>
     </row>
@@ -661,34 +561,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Introduction to Computer Science Principles II</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Introduction to Computer Science Principles II</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Liz Roberts-Kirchhoff (Primary)
-Terry Laesser</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
           <t>Monday-Tuesday-Wednesday-Thursday-Friday , 12:39 PM - 01:34 PM</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>25 of 35 seats remain.</t>
         </is>
       </c>
     </row>
@@ -700,33 +583,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Introduction to Computer Science Principles II</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Introduction to Computer Science Principles II</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Andrew Lapetina (Primary)</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
           <t>Monday-Tuesday-Wednesday-Thursday-Friday , 11:15 AM - 12:15 PM</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>27 of 35 seats remain.</t>
         </is>
       </c>
     </row>
@@ -738,33 +605,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Introduction to Computer Science Principles II</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Introduction to Computer Science Principles II</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Joshua Cormier (Primary)</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
           <t>Monday-Tuesday-Wednesday-Thursday-Friday , 08:00 AM - 08:45 AM</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>6 of 20 seats remain.</t>
         </is>
       </c>
     </row>
@@ -776,33 +627,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Introduction to Programming I</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Introduction to Programming I</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Mina Maleki (Primary)</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
           <t>Tuesday-Thursday , 11:20 AM - 12:35 PM</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>16 of 30 seats remain.</t>
         </is>
       </c>
     </row>
@@ -814,34 +649,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Programming I Laboratory</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Programming I Laboratory</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Mina Maleki (Primary)</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
           <t>Tuesday , 05:15 PM - 06:30 PM</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>FULL: 0 of 12 seats remain.
-8 of 8 waitlist seats remain.</t>
         </is>
       </c>
     </row>
@@ -853,31 +671,19 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Programming I Laboratory</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Programming I Laboratory</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Hebah Alquran (Primary)</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>18 of 20 seats remain.</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr"/>
+          <t>Wednesday-Thursday , 09:00 AM - 10:15 AM</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -887,37 +693,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>Introduction to Programming II</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>['1710,C']</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Catalog Prerequisites
-Area Prerequisites
-Prerequisites:Prereq(s) for CSSE1720 are:
- Course or Test: Comp Sci/Software Engineering 1710 
- Minimum Grade of C
- May not be taken concurrently. </t>
-        </is>
-      </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Introduction to Programming II</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Shadi Elaiyan Bani Taan (Primary)</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
           <t>Monday-Wednesday , 12:30 PM - 01:45 PM</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>4 of 20 seats remain.</t>
         </is>
       </c>
     </row>
@@ -929,38 +715,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>Introduction to Programming II</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>['1710,C']</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Catalog Prerequisites
-Area Prerequisites
-Prerequisites:Prereq(s) for CSSE1720 are:
- Course or Test: Comp Sci/Software Engineering 1710 
- Minimum Grade of C
- May not be taken concurrently. </t>
-        </is>
-      </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Introduction to Programming II</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Raef Aidibi (Primary)</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
           <t>Monday-Wednesday , 12:30 PM - 01:45 PM</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>8 of 24 seats remain.
-10 of 10 waitlist seats remain.</t>
         </is>
       </c>
     </row>
@@ -972,37 +737,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>Introduction to Programming II</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>['1710,C']</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Catalog Prerequisites
-Area Prerequisites
-Prerequisites:Prereq(s) for CSSE1720 are:
- Course or Test: Comp Sci/Software Engineering 1710 
- Minimum Grade of C
- May not be taken concurrently. </t>
-        </is>
-      </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Introduction to Programming II</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Ahmad Aljaafreh (Primary)</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
           <t>Monday-Wednesday , 08:00 AM - 10:00 AM</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>FULL: 0 of 100 seats remain.</t>
         </is>
       </c>
     </row>
@@ -1014,37 +759,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>Introduction to Programming II</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>['1710,C']</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Catalog Prerequisites
-Area Prerequisites
-Prerequisites:Prereq(s) for CSSE1720 are:
- Course or Test: Comp Sci/Software Engineering 1710 
- Minimum Grade of C
- May not be taken concurrently. </t>
-        </is>
-      </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Introduction to Programming II</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Ahmad Aljaafreh (Primary)</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
           <t>Tuesday-Thursday , 07:00 PM - 09:45 PM</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>31 of 100 seats remain.</t>
         </is>
       </c>
     </row>
@@ -1056,34 +781,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Programming II Laboratory</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Programming II Laboratory</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Shadi Elaiyan Bani Taan (Primary)</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
           <t>Wednesday , 02:00 PM - 03:15 PM</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>1 of 13 seats remain.
-5 of 5 waitlist seats remain.</t>
         </is>
       </c>
     </row>
@@ -1095,34 +803,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Programming II Laboratory</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Programming II Laboratory</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Shadi Elaiyan Bani Taan (Primary)</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
           <t>Monday , 02:00 PM - 03:15 PM</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>3 of 13 seats remain.
-5 of 5 waitlist seats remain.</t>
         </is>
       </c>
     </row>
@@ -1134,45 +825,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>Database Systems and Programming</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
           <t>['1720,C', 'or', '1722,C']</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Catalog Prerequisites
-Area Prerequisites
-Prerequisites:Prereq(s) for CSSE3540 are:
-(
- Course or Test: Comp Sci/Software Engineering 1720 
- Minimum Grade of C
- May not be taken concurrently. 
-)
-or
-(
- Course or Test: Comp Sci/Software Engineering 1722 
- Minimum Grade of C
- May not be taken concurrently. 
-)</t>
-        </is>
-      </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Database Systems and Programming</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Mina Maleki (Primary)</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
           <t>Tuesday-Thursday , 02:00 PM - 03:15 PM</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>7 of 20 seats remain.</t>
         </is>
       </c>
     </row>
@@ -1184,45 +847,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>Web Technology</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
           <t>['1720,C', 'or', '1722,C']</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Catalog Prerequisites
-Area Prerequisites
-Prerequisites:Prereq(s) for CSSE4440 are:
-(
- Course or Test: Comp Sci/Software Engineering 1720 
- Minimum Grade of C
- May not be taken concurrently. 
-)
-or
-(
- Course or Test: Comp Sci/Software Engineering 1722 
- Minimum Grade of C
- May not be taken concurrently. 
-)</t>
-        </is>
-      </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Web Technology</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Omid Aghili (Primary)</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
           <t>Monday-Wednesday , 01:30 PM - 04:45 PM</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>43 of 100 seats remain.</t>
         </is>
       </c>
     </row>
@@ -1234,37 +869,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>Operating Systems</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>['3430,C']</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Catalog Prerequisites
-Area Prerequisites
-Prerequisites:Prereq(s) for CSSE4490 are:
- Course or Test: Comp Sci/Software Engineering 3430 
- Minimum Grade of C
- May not be taken concurrently. </t>
-        </is>
-      </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Operating Systems</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Abhijit Dasgupta (Primary)</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
           <t>Monday-Wednesday , 05:15 PM - 06:30 PM</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>24 of 34 seats remain.</t>
         </is>
       </c>
     </row>
@@ -1276,33 +891,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Computer Security</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Computer Security</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Omid Aghili (Primary)</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
           <t>Tuesday-Thursday , 01:30 PM - 04:45 PM</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>43 of 100 seats remain.</t>
         </is>
       </c>
     </row>
@@ -1314,37 +913,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>Introduction to Artificial Intelligence</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
           <t>['3430,C']</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Catalog Prerequisites
-Area Prerequisites
-Prerequisites:Prereq(s) for CSSE4550 are:
- Course or Test: Comp Sci/Software Engineering 3430 
- Minimum Grade of C
- May not be taken concurrently. </t>
-        </is>
-      </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Introduction to Artificial Intelligence</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Shadi Elaiyan Bani Taan (Primary)</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
           <t>Monday-Wednesday , 11:00 AM - 12:15 PM</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>14 of 20 seats remain.</t>
         </is>
       </c>
     </row>
@@ -1356,37 +935,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>Introduction to Artificial Intelligence</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>['3430,C']</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Catalog Prerequisites
-Area Prerequisites
-Prerequisites:Prereq(s) for CSSE4550 are:
- Course or Test: Comp Sci/Software Engineering 3430 
- Minimum Grade of C
- May not be taken concurrently. </t>
-        </is>
-      </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Introduction to Artificial Intelligence</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Omid Aghili (Primary)</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
           <t>Tuesday-Thursday , 06:00 PM - 08:55 PM</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>42 of 100 seats remain.</t>
         </is>
       </c>
     </row>
@@ -1398,35 +957,19 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>Software Project Management</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
           <t>['4150,C']</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Catalog Prerequisites
-Area Prerequisites
-Prerequisites:Prereq(s) for CSSE4570 are
- Course or Test: Comp Sci/Software Engineering 4150 
- Minimum Grade of C
- May not be taken concurrently. </t>
-        </is>
-      </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Software Project Management</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Kevin Daimi (Primary)</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>14 of 25 seats remain.</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr"/>
+          <t>Tuesday-Thursday , 05:15 PM - 06:30 PM</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1436,33 +979,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Game Design, Develop, &amp; Tools</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Game Design, Develop, &amp; Tools</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Steven Rice (Primary)</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
           <t>Monday-Wednesday , 02:00 PM - 03:15 PM</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>FULL: 0 of 20 seats remain.</t>
         </is>
       </c>
     </row>
@@ -1474,37 +1001,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>Senior Design Project II</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
           <t>['4951,C']</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Catalog Prerequisites
-Area Prerequisites
-Prerequisites:Prereq(s) for CSSE4952 are:
- Course or Test: Comp Sci/Software Engineering 4951 
- Minimum Grade of C
- May not be taken concurrently. </t>
-        </is>
-      </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Senior Design Project II</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Shadi Elaiyan Bani Taan (Primary)</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
           <t>Monday-Wednesday , 09:00 AM - 10:15 AM</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>13 of 20 seats remain.</t>
         </is>
       </c>
     </row>
@@ -1516,33 +1023,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Artificial Intelligence</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Artificial Intelligence</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Shadi Elaiyan Bani Taan (Primary)</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
           <t>Monday-Wednesday , 11:00 AM - 12:15 PM</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>8 of 20 seats remain.</t>
         </is>
       </c>
     </row>
@@ -1554,31 +1045,19 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Architectures for Software Systems</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Architectures for Software Systems</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Rita Barrios (Primary)</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>18 of 25 seats remain.</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr"/>
+          <t>Monday , 06:40 PM - 09:10 PM</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1588,33 +1067,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Software Requirements Engineering</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Software Requirements Engineering</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Mina Maleki (Primary)</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
           <t>Tuesday-Thursday , 03:30 PM - 04:45 PM</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>14 of 20 seats remain.</t>
         </is>
       </c>
     </row>
@@ -1626,31 +1089,19 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Software Systems Project Management</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Software Systems Project Management</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Kevin Daimi (Primary)</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>22 of 25 seats remain.</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr"/>
+          <t>Tuesday-Thursday , 05:15 PM - 06:30 PM</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1660,33 +1111,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Graduate Design Project</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Catalog Prerequisites
-No prerequisite information available.</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Graduate Design Project</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Shadi Elaiyan Bani Taan (Primary)</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
           <t xml:space="preserve"> , -</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>1 of 5 seats remain.</t>
         </is>
       </c>
     </row>

</xml_diff>